<commit_message>
Updated Extra mile and Tradeling exceel file
</commit_message>
<xml_diff>
--- a/The extra mile/Tradeling.xlsx
+++ b/The extra mile/Tradeling.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sk/Documents/Tradeling/Functional-Test-cases/The extra mile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B5206F-C75F-8E43-9D2A-E000F23D8B0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7227DC5-2F33-D343-9739-27E5EF3F40E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="28040" windowHeight="16620" activeTab="1" xr2:uid="{E045BB90-203E-2940-A39E-16C19149C5EF}"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="28040" windowHeight="16620" activeTab="7" xr2:uid="{E045BB90-203E-2940-A39E-16C19149C5EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Buy Flow" sheetId="2" r:id="rId1"/>
-    <sheet name="Seller" sheetId="3" r:id="rId2"/>
-    <sheet name="General Test Cases" sheetId="4" r:id="rId3"/>
-    <sheet name="Testing Types" sheetId="5" r:id="rId4"/>
-    <sheet name="Homepage" sheetId="6" r:id="rId5"/>
-    <sheet name="PDP" sheetId="8" r:id="rId6"/>
-    <sheet name="Recommendation" sheetId="7" r:id="rId7"/>
+    <sheet name="SLP Search listing Page" sheetId="9" r:id="rId2"/>
+    <sheet name="Seller" sheetId="3" r:id="rId3"/>
+    <sheet name="General Test Cases" sheetId="4" r:id="rId4"/>
+    <sheet name="Testing Types" sheetId="5" r:id="rId5"/>
+    <sheet name="Homepage" sheetId="6" r:id="rId6"/>
+    <sheet name="PDP Product listing page" sheetId="8" r:id="rId7"/>
+    <sheet name="Recommendation" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>Product Buy Flow – Test cases</t>
   </si>
@@ -426,30 +427,9 @@
     <t>Homepage Test Cases</t>
   </si>
   <si>
-    <t>Is the page going to auto-scroll, and at what interval will the images be refreshed?</t>
-  </si>
-  <si>
-    <t>When the customer hovers over it, is it going to scroll to the next one?</t>
-  </si>
-  <si>
-    <t>When clicked on, is it taking the customer to the right page and right product deal?</t>
-  </si>
-  <si>
-    <t>Is the loading speed acceptable?</t>
-  </si>
-  <si>
-    <t>Can the rest of the content be viewed effortlessly, including newsletters, banners, social media links in the site footer, etc.?</t>
-  </si>
-  <si>
-    <t>Does the homepage appear the same way in different browsers and screen resolutions?</t>
-  </si>
-  <si>
     <t>Check if the recommendations given to customers are of relevant products that will interest the client</t>
   </si>
   <si>
-    <t>Are the recommendations showing on the page immediately after the client confirms the order they have made?</t>
-  </si>
-  <si>
     <t>Verify See all functionality once user click on it from PDP or from Homepage</t>
   </si>
   <si>
@@ -474,15 +454,6 @@
     <t>Verify the price of the product is displayed</t>
   </si>
   <si>
-    <t>Verify  delivery options are displayed</t>
-  </si>
-  <si>
-    <t>Verify  shipping information is displayed</t>
-  </si>
-  <si>
-    <t>Verify the review section is functioning.</t>
-  </si>
-  <si>
     <t>Verify Out of stock or In stock, information is showing on the page.</t>
   </si>
   <si>
@@ -499,6 +470,120 @@
   </si>
   <si>
     <t>Verify that the different pre-paid methods "COD/CC/DC/BANK TRANSFERESCROW" of payments are working fine.</t>
+  </si>
+  <si>
+    <t>Search Box Test Cases</t>
+  </si>
+  <si>
+    <t>Check if the search box is present or not.</t>
+  </si>
+  <si>
+    <t>Check if the search box length is as per the specification.</t>
+  </si>
+  <si>
+    <t>Check the length of the query to be added into the search box.</t>
+  </si>
+  <si>
+    <t>Check the characters allowed to be entered into the search box.</t>
+  </si>
+  <si>
+    <t>Check if the amazon page offers default focus at search box or not.</t>
+  </si>
+  <si>
+    <t>Search History Test Cases</t>
+  </si>
+  <si>
+    <t>Verify  payment options are displayed</t>
+  </si>
+  <si>
+    <t>Verify  seller information is displayed</t>
+  </si>
+  <si>
+    <t>Verify Shipping &amp; Stock details information are displayed</t>
+  </si>
+  <si>
+    <t>Verify the product details &amp; Company overview section</t>
+  </si>
+  <si>
+    <t>Verify Add to cart feature is displaying or not</t>
+  </si>
+  <si>
+    <t>Does all categories rails and Homepage banners are loading</t>
+  </si>
+  <si>
+    <t>Does the search box shows search page without any search query</t>
+  </si>
+  <si>
+    <t>What does search page shows if you enter nothing in search box and hit enter or press finder icon</t>
+  </si>
+  <si>
+    <t>What does search box does if the search query is not entered</t>
+  </si>
+  <si>
+    <t>Does the search box offers typo corrections for the search query</t>
+  </si>
+  <si>
+    <t>Does the search box presents auto suggestions when the query is being typed</t>
+  </si>
+  <si>
+    <t>Does the search box allows searching with incorrect spellings</t>
+  </si>
+  <si>
+    <t>Does the search history page keeps history of your previously searched products on amazon</t>
+  </si>
+  <si>
+    <t>Does the search history page offers you option to hide the history of previously searched products</t>
+  </si>
+  <si>
+    <t>Does the search history page offers matching products related to the search keywords</t>
+  </si>
+  <si>
+    <t>Does the search history page allows you to disable tracking the search completely</t>
+  </si>
+  <si>
+    <t>Does disabling search history makes any change to the suggestions offered by search-box</t>
+  </si>
+  <si>
+    <t>Does disabling search history stops certain products being featured</t>
+  </si>
+  <si>
+    <t>Does disabling search history reverts back to the default setting in a new session</t>
+  </si>
+  <si>
+    <t>Is the page going to auto-scroll, and at what interval will the images be refreshed</t>
+  </si>
+  <si>
+    <t>When the customer hovers over it, is it going to scroll to the next one</t>
+  </si>
+  <si>
+    <t>When clicked on, is it taking the customer to the right page and right product deal</t>
+  </si>
+  <si>
+    <t>Is the loading speed acceptable</t>
+  </si>
+  <si>
+    <t>Can the rest of the content be viewed effortlessly, including newsletters, banners, social media links in the site footer, etc.</t>
+  </si>
+  <si>
+    <t>Does the homepage appear the same way in different browsers and screen resolutions</t>
+  </si>
+  <si>
+    <t>Are the recommendations showing on the page immediately after the client confirms the order they have made</t>
+  </si>
+  <si>
+    <t>Responsive Test Cases</t>
+  </si>
+  <si>
+    <t>Does the search box appears on mobile</t>
+  </si>
+  <si>
+    <t>Does the search box suggestions appear on mobile or tablet</t>
+  </si>
+  <si>
+    <t>Does the search box offers category selector on mobile or tablet</t>
+  </si>
+  <si>
+    <t>Does the search box offers drop-down menu on smaller devices</t>
   </si>
 </sst>
 </file>
@@ -924,10 +1009,13 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="185.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="37" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -956,7 +1044,7 @@
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1026,7 +1114,7 @@
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1046,17 +1134,17 @@
     </row>
     <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1065,14 +1153,160 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E0F57F-5B7E-0E4F-928A-5A7105774644}">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="124.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="37" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="37" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="37" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212D51D8-459B-894B-9208-3B82F7F863A1}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="162.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1228,15 +1462,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B72EC4-5CE8-134A-A5D9-D46F711DC7CB}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="130.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
@@ -1509,7 +1746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817B434D-EE85-264E-9F49-9EABDA02C3C1}">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -1736,15 +1973,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA579B95-1F54-3343-BB5E-4EF27DCCE476}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="140.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
@@ -1753,7 +1993,7 @@
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1764,7 +2004,7 @@
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1775,7 +2015,7 @@
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1786,7 +2026,7 @@
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1797,7 +2037,7 @@
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1808,7 +2048,7 @@
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1817,64 +2057,9 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8998FC-FB33-D045-B2ED-D1E516DD9B94}">
-  <dimension ref="A1:A9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="38" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>92</v>
+    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1883,26 +2068,100 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9364023-C589-1E4E-AFEB-E1C7316F82BB}">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8998FC-FB33-D045-B2ED-D1E516DD9B94}">
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="82.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="38" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9364023-C589-1E4E-AFEB-E1C7316F82BB}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="129.6640625" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1915,7 +2174,7 @@
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1928,7 +2187,7 @@
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1938,7 +2197,7 @@
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>